<commit_message>
edit Excel pandas op
</commit_message>
<xml_diff>
--- a/pycode/file/20210806_Tn.xlsx
+++ b/pycode/file/20210806_Tn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\TOSHIBA_EXT\data\programming\tool\pycode\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2946951F-B3C8-4AAC-89EF-0AA454F30160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE6599-2BBA-450B-8D63-DA51DC54F27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38415" yWindow="390" windowWidth="15255" windowHeight="9623" xr2:uid="{3E2D7707-D2B1-430B-97F7-A6EB33D6B345}"/>
+    <workbookView xWindow="45368" yWindow="375" windowWidth="17032" windowHeight="13695" xr2:uid="{3E2D7707-D2B1-430B-97F7-A6EB33D6B345}"/>
   </bookViews>
   <sheets>
     <sheet name="Joint Displacements" sheetId="1" r:id="rId1"/>
@@ -676,7 +676,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -698,6 +698,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -783,6 +789,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,8 +1107,8 @@
   <dimension ref="A1:Q163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="3" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A163" sqref="A163:XFD163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7567,12 +7574,12 @@
         <v>7.9988949675000017E-6</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="K163">
+    <row r="163" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="K163" s="15">
         <f>SUM(K4:K162)</f>
         <v>9.5068760030999986</v>
       </c>
-      <c r="L163">
+      <c r="L163" s="15">
         <f>SUM(L4:L162)</f>
         <v>7.8818298369439516E-2</v>
       </c>

</xml_diff>

<commit_message>
add fii in all NaN and column NaN ability
</commit_message>
<xml_diff>
--- a/pycode/file/20210806_Tn.xlsx
+++ b/pycode/file/20210806_Tn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\data\programming\tool\pycode\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E46FE5C-DEA5-4CAA-AD86-8E8391757103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8070E8A3-4B04-47A1-B12D-2A367FEF985B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10913" windowWidth="12960" windowHeight="10687" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10275" windowWidth="12960" windowHeight="10688" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -154,6 +154,10 @@
   </si>
   <si>
     <t>yes</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>gary01</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -390,11 +394,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1566,11 +1570,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1" t="s">
@@ -1633,7 +1637,7 @@
   <dimension ref="A1:D164"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1649,7 +1653,9 @@
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
@@ -1659,7 +1665,7 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>